<commit_message>
fixed initial questions + fuzzywuzzy
to add:
- llm extractions prior to fuzzywuzzy
- the queries
- loop mechanism
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JU\Knowledge_Representation_HT2024\project\TO_BE_NAMED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0583DEBE-6280-4E3F-9E85-8C376F45C912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBD82FE-ECCC-4D3A-A20F-B95DF668D257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="19360" windowHeight="10960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ID</t>
   </si>
@@ -72,6 +72,15 @@
   </si>
   <si>
     <t>Workflow Diagram, Milestones, Project Tools</t>
+  </si>
+  <si>
+    <t>Reviewed Queries, Models, and Project Load Ahead</t>
+  </si>
+  <si>
+    <t>ma, is, se, cl, ce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reviewed Model &amp; UI, Planned to write more on Overleaf &amp; Get An MVP </t>
   </si>
 </sst>
 </file>
@@ -434,14 +443,14 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.6328125" customWidth="1"/>
     <col min="2" max="2" width="27.26953125" customWidth="1"/>
-    <col min="3" max="3" width="33.08984375" customWidth="1"/>
+    <col min="3" max="3" width="62.7265625" customWidth="1"/>
     <col min="4" max="4" width="27.36328125" customWidth="1"/>
     <col min="5" max="5" width="22.81640625" customWidth="1"/>
   </cols>
@@ -485,6 +494,15 @@
       <c r="A3">
         <v>2</v>
       </c>
+      <c r="B3" s="6">
+        <v>45646</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
       <c r="E3" t="s">
         <v>5</v>
       </c>
@@ -492,6 +510,12 @@
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
+      </c>
+      <c r="B4" s="6">
+        <v>45651</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
       </c>
       <c r="E4" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
added radio buttons and loops
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JU\Knowledge_Representation_HT2024\project\TO_BE_NAMED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBD82FE-ECCC-4D3A-A20F-B95DF668D257}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005C7BAD-5065-4C9F-BE37-3800D80B1AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>ID</t>
   </si>
@@ -81,6 +81,9 @@
   </si>
   <si>
     <t xml:space="preserve">Reviewed Model &amp; UI, Planned to write more on Overleaf &amp; Get An MVP </t>
+  </si>
+  <si>
+    <t>Updated everyone on current project progress, planned work for weekend, more functionality and write on the report</t>
   </si>
 </sst>
 </file>
@@ -443,14 +446,14 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.6328125" customWidth="1"/>
     <col min="2" max="2" width="27.26953125" customWidth="1"/>
-    <col min="3" max="3" width="62.7265625" customWidth="1"/>
+    <col min="3" max="3" width="99.1796875" customWidth="1"/>
     <col min="4" max="4" width="27.36328125" customWidth="1"/>
     <col min="5" max="5" width="22.81640625" customWidth="1"/>
   </cols>
@@ -517,6 +520,9 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
+      <c r="D4" t="s">
+        <v>13</v>
+      </c>
       <c r="E4" t="s">
         <v>6</v>
       </c>
@@ -524,6 +530,15 @@
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" s="6">
+        <v>45653</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
updated excel meetings tab
</commit_message>
<xml_diff>
--- a/meetings.xlsx
+++ b/meetings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JU\Knowledge_Representation_HT2024\project\TO_BE_NAMED\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005C7BAD-5065-4C9F-BE37-3800D80B1AB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F320CC-1D77-42AD-8F88-DEDCCC42B07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>ID</t>
   </si>
@@ -84,6 +84,12 @@
   </si>
   <si>
     <t>Updated everyone on current project progress, planned work for weekend, more functionality and write on the report</t>
+  </si>
+  <si>
+    <t>Discussed current progress on Chat Profiles, divided up the work, and planned for the report writing.</t>
+  </si>
+  <si>
+    <t>Reviewed current work, Suggest Updates to One of the Chats, Planned Remaining Report Writing</t>
   </si>
 </sst>
 </file>
@@ -446,7 +452,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -548,6 +554,15 @@
       <c r="A6">
         <v>5</v>
       </c>
+      <c r="B6" s="6">
+        <v>45659</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
       <c r="E6" t="s">
         <v>7</v>
       </c>
@@ -555,6 +570,15 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
+      </c>
+      <c r="B7" s="6">
+        <v>45664</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>